<commit_message>
06-07-2018 Pago Pro v1
</commit_message>
<xml_diff>
--- a/public/uploads/formato.xlsx
+++ b/public/uploads/formato.xlsx
@@ -32,30 +32,6 @@
     <author>Usuario de Windows</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Usuario de Windows:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Correo Eléctronico que se logea al sistema</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
@@ -149,6 +125,54 @@
           </rPr>
           <t xml:space="preserve">
 Debe ser el mismo nombre que aparece en el Sistema</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Usuario de Windows:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>El registro de Descartará si se encuentra en el Sistema</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Usuario de Windows:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+El nombre del correo debe estar en el mantenedor de correos, ya que se incorporará automaticamente</t>
         </r>
       </text>
     </comment>
@@ -157,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>CONDICION</t>
   </si>
@@ -223,6 +247,9 @@
   </si>
   <si>
     <t>Dpto</t>
+  </si>
+  <si>
+    <t>Correo Tipo</t>
   </si>
 </sst>
 </file>
@@ -233,7 +260,7 @@
     <numFmt numFmtId="164" formatCode="[$$-340A]#,##0"/>
     <numFmt numFmtId="165" formatCode="_ [$$-340A]* #,##0.00_ ;_ [$$-340A]* \-#,##0.00_ ;_ [$$-340A]* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,6 +310,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -649,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V9"/>
+  <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +720,7 @@
     <col min="23" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -747,8 +787,11 @@
       <c r="V1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="L9" s="15"/>
     </row>
   </sheetData>

</xml_diff>